<commit_message>
Second Commit - Changes to add red/blue graph lines
</commit_message>
<xml_diff>
--- a/src/model_results.xlsx
+++ b/src/model_results.xlsx
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.487188277561616</v>
+        <v>8.208056818716059</v>
       </c>
       <c r="C3" t="n">
-        <v>8.585832366216417</v>
+        <v>9.971559878739022</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.803904050613974</v>
+        <v>10.44380567568414</v>
       </c>
       <c r="C4" t="n">
-        <v>7.692517573181676</v>
+        <v>12.37385914388238</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.258390245919528</v>
+        <v>5.221453118045278</v>
       </c>
       <c r="C5" t="n">
-        <v>7.006439660921402</v>
+        <v>6.975666183484694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>